<commit_message>
Su + steering (en cours)
</commit_message>
<xml_diff>
--- a/ST - Steering System/Cost/Cost_steering_le_bon_ABR avec noms.xlsx
+++ b/ST - Steering System/Cost/Cost_steering_le_bon_ABR avec noms.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10452"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10452" firstSheet="29" activeTab="36"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="33" r:id="rId1"/>
@@ -39,9 +39,15 @@
     <sheet name="ST 04001" sheetId="30" r:id="rId30"/>
     <sheet name="ST 04002" sheetId="31" r:id="rId31"/>
     <sheet name="ST 04002 Drawing" sheetId="32" r:id="rId32"/>
+    <sheet name="ST A0500" sheetId="36" r:id="rId33"/>
+    <sheet name="ST 05001" sheetId="37" r:id="rId34"/>
+    <sheet name="ST 05002" sheetId="40" r:id="rId35"/>
+    <sheet name="dST 05002" sheetId="42" r:id="rId36"/>
+    <sheet name="ST 05003" sheetId="41" r:id="rId37"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId33"/>
+    <externalReference r:id="rId38"/>
+    <externalReference r:id="rId39"/>
   </externalReferences>
   <definedNames>
     <definedName name="BR_01001_f">'[1]ST Part 1'!$J$27</definedName>
@@ -132,9 +138,21 @@
     <definedName name="ST_03003_m">'ST 03003'!$N$12</definedName>
     <definedName name="ST_03003_p">'ST 03003'!$I$19</definedName>
     <definedName name="ST_03003_q">'ST 03003'!$N$3</definedName>
+    <definedName name="ST_04001" localSheetId="33">'ST 05001'!$B$6</definedName>
+    <definedName name="ST_04001" localSheetId="34">'ST 05002'!$B$6</definedName>
+    <definedName name="ST_04001" localSheetId="36">'ST 05003'!$B$6</definedName>
     <definedName name="ST_04001">'ST 04001'!$B$6</definedName>
+    <definedName name="ST_04001_m" localSheetId="33">'ST 05001'!$N$12</definedName>
+    <definedName name="ST_04001_m" localSheetId="34">'ST 05002'!$N$12</definedName>
+    <definedName name="ST_04001_m" localSheetId="36">'ST 05003'!$N$11</definedName>
     <definedName name="ST_04001_m">'ST 04001'!$N$15</definedName>
+    <definedName name="ST_04001_p" localSheetId="33">'ST 05001'!$I$16</definedName>
+    <definedName name="ST_04001_p" localSheetId="34">'ST 05002'!$I$20</definedName>
+    <definedName name="ST_04001_p" localSheetId="36">'ST 05003'!$I$14</definedName>
     <definedName name="ST_04001_p">'ST 04001'!$I$24</definedName>
+    <definedName name="ST_04001_q" localSheetId="33">'ST 05001'!$N$3</definedName>
+    <definedName name="ST_04001_q" localSheetId="34">'ST 05002'!$N$3</definedName>
+    <definedName name="ST_04001_q" localSheetId="36">'ST 05003'!$N$3</definedName>
     <definedName name="ST_04001_q">'ST 04001'!$N$3</definedName>
     <definedName name="ST_04002">'ST 04002'!$B$6</definedName>
     <definedName name="ST_04002_m">'ST 04002'!$N$12</definedName>
@@ -157,18 +175,24 @@
     <definedName name="ST_A0300_m">'ST A0300'!$N$18</definedName>
     <definedName name="ST_A0300_p">'ST A0300'!$I$23</definedName>
     <definedName name="ST_A0300_q">'ST A0300'!$N$3</definedName>
+    <definedName name="ST_A0400" localSheetId="32">'ST A0500'!$B$5</definedName>
     <definedName name="ST_A0400">'ST A0400'!$B$5</definedName>
+    <definedName name="ST_A0400_f" localSheetId="32">'ST A0500'!$J$46</definedName>
     <definedName name="ST_A0400_f">'ST A0400'!$J$22</definedName>
+    <definedName name="ST_A0400_p" localSheetId="32">'ST A0500'!$I$38</definedName>
     <definedName name="ST_A0400_p">'ST A0400'!$I$17</definedName>
+    <definedName name="ST_A0400_q" localSheetId="32">'ST A0500'!$N$3</definedName>
     <definedName name="ST_A0400_q">'ST A0400'!$N$3</definedName>
+    <definedName name="SU_12001_q">'[2]SU 12001'!$N$3</definedName>
+    <definedName name="SU_12002_q">'[2]SU 12002'!$N$3</definedName>
+    <definedName name="SU_12003_q">'[2]SU 12003'!$N$3</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2069" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2384" uniqueCount="406">
   <si>
     <t>University</t>
   </si>
@@ -1224,13 +1248,175 @@
   </si>
   <si>
     <t>ST 04001</t>
+  </si>
+  <si>
+    <t>ST A0500</t>
+  </si>
+  <si>
+    <t>Steering rod</t>
+  </si>
+  <si>
+    <t>Steering rod, right and left are symetric</t>
+  </si>
+  <si>
+    <t>Steering rod tube</t>
+  </si>
+  <si>
+    <t>Steering rod insert</t>
+  </si>
+  <si>
+    <t>Rod End, Industrial</t>
+  </si>
+  <si>
+    <t>Right-hand rod end for pushrod extremities</t>
+  </si>
+  <si>
+    <t>Balls Diameter</t>
+  </si>
+  <si>
+    <t>Left-hand rod end for pushrod extremities</t>
+  </si>
+  <si>
+    <t>Hand Finish - Surface Preperation</t>
+  </si>
+  <si>
+    <t>Solvent degreasing  on carbon tube</t>
+  </si>
+  <si>
+    <t>cm²</t>
+  </si>
+  <si>
+    <t>Solvent degreasing  on insert</t>
+  </si>
+  <si>
+    <t>Brush apply</t>
+  </si>
+  <si>
+    <t>Glue insert to pushrod tube</t>
+  </si>
+  <si>
+    <t>Hand - Start Only</t>
+  </si>
+  <si>
+    <t>Put a nut on the rod end</t>
+  </si>
+  <si>
+    <t>Hand, Loose &lt;= 25.4 mm</t>
+  </si>
+  <si>
+    <t>Screwing by hand the rod end in the pullrod insert</t>
+  </si>
+  <si>
+    <t>Thighten the M8 nuts</t>
+  </si>
+  <si>
+    <t>Reaction tool &lt;= 25.4 mm</t>
+  </si>
+  <si>
+    <t>Assemble, 1kg, Loose</t>
+  </si>
+  <si>
+    <t>Put the spacers of the rocker in place</t>
+  </si>
+  <si>
+    <t>Put the washers of the rocker in place</t>
+  </si>
+  <si>
+    <t>Bolt pullrod into the rocker</t>
+  </si>
+  <si>
+    <t>Put the spacers of the A-arm in place</t>
+  </si>
+  <si>
+    <t>Put the washers of the A-arm in place</t>
+  </si>
+  <si>
+    <t>Bolt pullrod into the A-Arm</t>
+  </si>
+  <si>
+    <t>Put the nuts into the bolts</t>
+  </si>
+  <si>
+    <t>Bolt,Grade 8.8 (SAE)</t>
+  </si>
+  <si>
+    <t>Pullrod to rocker fixing bolt</t>
+  </si>
+  <si>
+    <t>Pullrod to A-arm fixing bolt</t>
+  </si>
+  <si>
+    <t>To tighten the rod ends</t>
+  </si>
+  <si>
+    <t>To tighten the bolts</t>
+  </si>
+  <si>
+    <t>ST 05001</t>
+  </si>
+  <si>
+    <t>ST 05002</t>
+  </si>
+  <si>
+    <t>ST 05003</t>
+  </si>
+  <si>
+    <t>Spacer</t>
+  </si>
+  <si>
+    <t>Carbon fiber, 1 Ply</t>
+  </si>
+  <si>
+    <t>Stock material</t>
+  </si>
+  <si>
+    <t>Round area, diameter 16x2 mm</t>
+  </si>
+  <si>
+    <t>Lamination, Filament Wirring</t>
+  </si>
+  <si>
+    <t>Tube lamination</t>
+  </si>
+  <si>
+    <t>Aluminium, Premium (per kg)</t>
+  </si>
+  <si>
+    <t>cylinder</t>
+  </si>
+  <si>
+    <t>Round area diam. 18mm</t>
+  </si>
+  <si>
+    <t>Setup for machining and removal</t>
+  </si>
+  <si>
+    <t>Material removal - side view profile</t>
+  </si>
+  <si>
+    <t>Machining setup, change</t>
+  </si>
+  <si>
+    <t>Setup for machining process</t>
+  </si>
+  <si>
+    <t>Tapping Holes</t>
+  </si>
+  <si>
+    <t>Rod End emplacement</t>
+  </si>
+  <si>
+    <t>2 parts from a single machine setup (tierod insert)</t>
+  </si>
+  <si>
+    <t>Drawing :</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="25">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="27">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
@@ -1256,8 +1442,10 @@
     <numFmt numFmtId="184" formatCode="#,##0.000"/>
     <numFmt numFmtId="185" formatCode="#,##0.000_ ;\-#,##0.000\ "/>
     <numFmt numFmtId="186" formatCode="_-* #,##0.000\ _€_-;\-* #,##0.000\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
+    <numFmt numFmtId="187" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00,;_-[$$-409]* \-??_ ;_-@_ "/>
+    <numFmt numFmtId="188" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1404,6 +1592,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="16">
     <fill>
@@ -1495,7 +1691,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="43">
     <border>
       <left/>
       <right/>
@@ -1800,8 +1996,227 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="9"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1831,8 +2246,14 @@
     <xf numFmtId="164" fontId="12" fillId="8" borderId="10">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="295">
+  <cellXfs count="395">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
@@ -2331,15 +2752,155 @@
     <xf numFmtId="11" fontId="14" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="19" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="9" xfId="20" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="9" xfId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="9" xfId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="9" xfId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="2" fillId="8" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="30" xfId="12" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="21" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="21" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="21" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="12" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="21" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="12" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="19" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="187" fontId="14" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="12" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="39" fontId="14" fillId="0" borderId="11" xfId="12" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
+    <xf numFmtId="37" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="7" fillId="0" borderId="41" xfId="19" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="38" xfId="19" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="40" xfId="19" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="41" xfId="19" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="188" fontId="7" fillId="0" borderId="41" xfId="19" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="41" xfId="19" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="178" fontId="7" fillId="0" borderId="41" xfId="19" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="11" fontId="7" fillId="0" borderId="41" xfId="19" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="184" fontId="7" fillId="0" borderId="41" xfId="19" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="41" xfId="19" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="42" xfId="19" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="21" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="188" fontId="14" fillId="0" borderId="2" xfId="21" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="21" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="14" fillId="0" borderId="2" xfId="12" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="19" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="21" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="2" xfId="20" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="2" xfId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="2" xfId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="21" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="11" fontId="7" fillId="0" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="37" xfId="21" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="21" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="21" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="41" xfId="24" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="8" fillId="0" borderId="2" xfId="21" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="21" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="21" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="21" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="21" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="2" xfId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="21" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="21" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="21" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="21" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="21" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="25">
     <cellStyle name="Comma 2" xfId="17"/>
     <cellStyle name="Cost Table Plain" xfId="18"/>
     <cellStyle name="Cost_Red" xfId="10"/>
     <cellStyle name="Cost_Yellow" xfId="9"/>
     <cellStyle name="Lien hypertexte" xfId="2" builtinId="8"/>
     <cellStyle name="Milliers 2" xfId="4"/>
+    <cellStyle name="Milliers 2 2" xfId="20"/>
     <cellStyle name="Milliers 3" xfId="15"/>
+    <cellStyle name="Milliers 3 4" xfId="23"/>
     <cellStyle name="Monétaire" xfId="1" builtinId="4"/>
     <cellStyle name="Monétaire 10" xfId="3"/>
     <cellStyle name="Monétaire 2" xfId="6"/>
@@ -2347,8 +2908,12 @@
     <cellStyle name="Neutre" xfId="8" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="13"/>
+    <cellStyle name="Normal 2 2 4 2 3" xfId="19"/>
+    <cellStyle name="Normal 2 2 4 3 2" xfId="24"/>
     <cellStyle name="Normal 3" xfId="16"/>
+    <cellStyle name="Normal 3 2 2" xfId="22"/>
     <cellStyle name="Normal 4" xfId="5"/>
+    <cellStyle name="Normal 4 2" xfId="21"/>
     <cellStyle name="Normal_Sheet1" xfId="7"/>
     <cellStyle name="Style 1" xfId="11"/>
     <cellStyle name="TableStyleLight1" xfId="12"/>
@@ -2358,6 +2923,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -3143,7 +3711,7 @@
         <xdr:cNvPr id="2" name="Image 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{944EA2C3-B977-45D4-917A-A561C5F5D9F9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{944EA2C3-B977-45D4-917A-A561C5F5D9F9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3319,6 +3887,113 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing28.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>356932</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1400-000030000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect r="2804"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="11544300" y="2257425"/>
+          <a:ext cx="1176082" cy="828675"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing29.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>306432</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>126819</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>382702</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11193507" y="2327094"/>
+          <a:ext cx="2047945" cy="1540056"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
@@ -3357,6 +4032,55 @@
         <a:xfrm>
           <a:off x="7604759" y="3101339"/>
           <a:ext cx="2969547" cy="2103561"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing30.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>53340</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>628651</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="email">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="53340" y="259080"/>
+          <a:ext cx="7707631" cy="5440680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3792,6 +4516,347 @@
 </externalLink>
 </file>
 
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="BOM"/>
+      <sheetName val="SU A0100"/>
+      <sheetName val="SU 01001"/>
+      <sheetName val="dSU 01001"/>
+      <sheetName val="SU 01002"/>
+      <sheetName val="dSU 01002"/>
+      <sheetName val="SU 01003"/>
+      <sheetName val="SU 01004"/>
+      <sheetName val="SU 01005"/>
+      <sheetName val="dSU 01005"/>
+      <sheetName val="SU 01006"/>
+      <sheetName val="dSU 01006"/>
+      <sheetName val="SU 01007"/>
+      <sheetName val="dSU 01007"/>
+      <sheetName val="SU 01008"/>
+      <sheetName val="dSU 01008"/>
+      <sheetName val="SU 01009"/>
+      <sheetName val="dSU 01009"/>
+      <sheetName val="SU 01010"/>
+      <sheetName val="dSU 01010"/>
+      <sheetName val="SU 01011"/>
+      <sheetName val="dSU 01011"/>
+      <sheetName val="SU A0200"/>
+      <sheetName val="SU 02001"/>
+      <sheetName val="dSU 02001"/>
+      <sheetName val="SU 02002"/>
+      <sheetName val="dSU 02002"/>
+      <sheetName val="SU 02003"/>
+      <sheetName val="SU 02004"/>
+      <sheetName val="SU 02005"/>
+      <sheetName val="dSU 02005"/>
+      <sheetName val="SU 02006"/>
+      <sheetName val="dSU 02006"/>
+      <sheetName val="SU 02007"/>
+      <sheetName val="dSU 02007"/>
+      <sheetName val="SU 02008"/>
+      <sheetName val="dSU 02008"/>
+      <sheetName val="SU 02009"/>
+      <sheetName val="dSU 02009"/>
+      <sheetName val="SU 02010"/>
+      <sheetName val="dSU 02010"/>
+      <sheetName val="SU 02011"/>
+      <sheetName val="dSU 02011"/>
+      <sheetName val="SU A0300"/>
+      <sheetName val="SU 03001"/>
+      <sheetName val="dSU 03001"/>
+      <sheetName val="SU 03002"/>
+      <sheetName val="dSU 03002"/>
+      <sheetName val="SU 03003"/>
+      <sheetName val="SU 03004"/>
+      <sheetName val="SU 03005"/>
+      <sheetName val="dSU 03005"/>
+      <sheetName val="SU 03006"/>
+      <sheetName val="dSU 03006"/>
+      <sheetName val="SU 03007"/>
+      <sheetName val="dSU 03007"/>
+      <sheetName val="SU 03008"/>
+      <sheetName val="dSU 03008"/>
+      <sheetName val="SU 03009"/>
+      <sheetName val="dSU 03009"/>
+      <sheetName val="SU 03010"/>
+      <sheetName val="dSU 03010"/>
+      <sheetName val="SU 03011"/>
+      <sheetName val="dSU 03011"/>
+      <sheetName val="SU A0400"/>
+      <sheetName val="SU 04001"/>
+      <sheetName val="dSU 04001"/>
+      <sheetName val="SU 04002"/>
+      <sheetName val="dSU 04002"/>
+      <sheetName val="SU 04003"/>
+      <sheetName val="SU 04004"/>
+      <sheetName val="SU 04005"/>
+      <sheetName val="dSU 04005"/>
+      <sheetName val="SU 04006"/>
+      <sheetName val="dSU 04006"/>
+      <sheetName val="SU 04007"/>
+      <sheetName val="dSU 04007"/>
+      <sheetName val="SU 04008"/>
+      <sheetName val="dSU 04008"/>
+      <sheetName val="SU 04009"/>
+      <sheetName val="dSU 04009"/>
+      <sheetName val="SU 04010"/>
+      <sheetName val="dSU 04010"/>
+      <sheetName val="SU 04011"/>
+      <sheetName val="dSU 04011"/>
+      <sheetName val="SU A0500"/>
+      <sheetName val="SU 05001"/>
+      <sheetName val="dSU 05001"/>
+      <sheetName val="SU A0600"/>
+      <sheetName val="SU 06001"/>
+      <sheetName val="SU 06002"/>
+      <sheetName val="SU 06003"/>
+      <sheetName val="dSU 06003"/>
+      <sheetName val="SU 06004"/>
+      <sheetName val="SU A0700"/>
+      <sheetName val="SU 07001"/>
+      <sheetName val="dSU 07001"/>
+      <sheetName val="SU A0800"/>
+      <sheetName val="SU 08001"/>
+      <sheetName val="SU 08002"/>
+      <sheetName val="dSU 08002"/>
+      <sheetName val="SU 08003"/>
+      <sheetName val="SU A0900"/>
+      <sheetName val="SU 09001"/>
+      <sheetName val="SU 09002"/>
+      <sheetName val="dSU 09002"/>
+      <sheetName val="SU 09003"/>
+      <sheetName val="dSU 09003"/>
+      <sheetName val="SU 09004"/>
+      <sheetName val="dSU 09004"/>
+      <sheetName val="SU A1000"/>
+      <sheetName val="SU 10001"/>
+      <sheetName val="dSU 10001"/>
+      <sheetName val="SU 10002"/>
+      <sheetName val="dSU 10002"/>
+      <sheetName val="SU 10003"/>
+      <sheetName val="dSU 10003"/>
+      <sheetName val="SU 10004"/>
+      <sheetName val="dSU 10004"/>
+      <sheetName val="SU 10005"/>
+      <sheetName val="dSU 10005"/>
+      <sheetName val="SU A1100 "/>
+      <sheetName val="SU 11001"/>
+      <sheetName val="dSU 11001"/>
+      <sheetName val="SU 11002"/>
+      <sheetName val="dSU 11002"/>
+      <sheetName val="SU 11003"/>
+      <sheetName val="dSU 11003"/>
+      <sheetName val="SU 11004"/>
+      <sheetName val="dSU 11004"/>
+      <sheetName val="SU A1200"/>
+      <sheetName val="SU 12001"/>
+      <sheetName val="SU 12002"/>
+      <sheetName val="dSU 12002"/>
+      <sheetName val="SU 12003"/>
+      <sheetName val="dSU 12003"/>
+      <sheetName val="SU 12004"/>
+      <sheetName val="dSU 12004"/>
+      <sheetName val="SU A1300"/>
+      <sheetName val="SU 13001"/>
+      <sheetName val="dSU 13001"/>
+      <sheetName val="SU 13002"/>
+      <sheetName val="dSU 13002"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="17" refreshError="1"/>
+      <sheetData sheetId="18" refreshError="1"/>
+      <sheetData sheetId="19" refreshError="1"/>
+      <sheetData sheetId="20" refreshError="1"/>
+      <sheetData sheetId="21" refreshError="1"/>
+      <sheetData sheetId="22" refreshError="1"/>
+      <sheetData sheetId="23" refreshError="1"/>
+      <sheetData sheetId="24" refreshError="1"/>
+      <sheetData sheetId="25" refreshError="1"/>
+      <sheetData sheetId="26" refreshError="1"/>
+      <sheetData sheetId="27" refreshError="1"/>
+      <sheetData sheetId="28" refreshError="1"/>
+      <sheetData sheetId="29" refreshError="1"/>
+      <sheetData sheetId="30" refreshError="1"/>
+      <sheetData sheetId="31" refreshError="1"/>
+      <sheetData sheetId="32" refreshError="1"/>
+      <sheetData sheetId="33" refreshError="1"/>
+      <sheetData sheetId="34" refreshError="1"/>
+      <sheetData sheetId="35" refreshError="1"/>
+      <sheetData sheetId="36" refreshError="1"/>
+      <sheetData sheetId="37" refreshError="1"/>
+      <sheetData sheetId="38" refreshError="1"/>
+      <sheetData sheetId="39" refreshError="1"/>
+      <sheetData sheetId="40" refreshError="1"/>
+      <sheetData sheetId="41" refreshError="1"/>
+      <sheetData sheetId="42" refreshError="1"/>
+      <sheetData sheetId="43" refreshError="1"/>
+      <sheetData sheetId="44" refreshError="1"/>
+      <sheetData sheetId="45" refreshError="1"/>
+      <sheetData sheetId="46" refreshError="1"/>
+      <sheetData sheetId="47" refreshError="1"/>
+      <sheetData sheetId="48" refreshError="1"/>
+      <sheetData sheetId="49" refreshError="1"/>
+      <sheetData sheetId="50" refreshError="1"/>
+      <sheetData sheetId="51" refreshError="1"/>
+      <sheetData sheetId="52" refreshError="1"/>
+      <sheetData sheetId="53" refreshError="1"/>
+      <sheetData sheetId="54" refreshError="1"/>
+      <sheetData sheetId="55" refreshError="1"/>
+      <sheetData sheetId="56" refreshError="1"/>
+      <sheetData sheetId="57" refreshError="1"/>
+      <sheetData sheetId="58" refreshError="1"/>
+      <sheetData sheetId="59" refreshError="1"/>
+      <sheetData sheetId="60" refreshError="1"/>
+      <sheetData sheetId="61" refreshError="1"/>
+      <sheetData sheetId="62" refreshError="1"/>
+      <sheetData sheetId="63" refreshError="1"/>
+      <sheetData sheetId="64" refreshError="1"/>
+      <sheetData sheetId="65" refreshError="1"/>
+      <sheetData sheetId="66" refreshError="1"/>
+      <sheetData sheetId="67" refreshError="1"/>
+      <sheetData sheetId="68" refreshError="1"/>
+      <sheetData sheetId="69" refreshError="1"/>
+      <sheetData sheetId="70" refreshError="1"/>
+      <sheetData sheetId="71" refreshError="1"/>
+      <sheetData sheetId="72" refreshError="1"/>
+      <sheetData sheetId="73" refreshError="1"/>
+      <sheetData sheetId="74" refreshError="1"/>
+      <sheetData sheetId="75" refreshError="1"/>
+      <sheetData sheetId="76" refreshError="1"/>
+      <sheetData sheetId="77" refreshError="1"/>
+      <sheetData sheetId="78" refreshError="1"/>
+      <sheetData sheetId="79" refreshError="1"/>
+      <sheetData sheetId="80" refreshError="1"/>
+      <sheetData sheetId="81" refreshError="1"/>
+      <sheetData sheetId="82" refreshError="1"/>
+      <sheetData sheetId="83" refreshError="1"/>
+      <sheetData sheetId="84" refreshError="1"/>
+      <sheetData sheetId="85" refreshError="1"/>
+      <sheetData sheetId="86" refreshError="1"/>
+      <sheetData sheetId="87" refreshError="1"/>
+      <sheetData sheetId="88" refreshError="1"/>
+      <sheetData sheetId="89" refreshError="1"/>
+      <sheetData sheetId="90" refreshError="1"/>
+      <sheetData sheetId="91" refreshError="1"/>
+      <sheetData sheetId="92" refreshError="1"/>
+      <sheetData sheetId="93" refreshError="1"/>
+      <sheetData sheetId="94" refreshError="1"/>
+      <sheetData sheetId="95" refreshError="1"/>
+      <sheetData sheetId="96" refreshError="1"/>
+      <sheetData sheetId="97" refreshError="1"/>
+      <sheetData sheetId="98" refreshError="1"/>
+      <sheetData sheetId="99" refreshError="1"/>
+      <sheetData sheetId="100" refreshError="1"/>
+      <sheetData sheetId="101" refreshError="1"/>
+      <sheetData sheetId="102" refreshError="1"/>
+      <sheetData sheetId="103" refreshError="1"/>
+      <sheetData sheetId="104" refreshError="1"/>
+      <sheetData sheetId="105" refreshError="1"/>
+      <sheetData sheetId="106" refreshError="1"/>
+      <sheetData sheetId="107" refreshError="1"/>
+      <sheetData sheetId="108" refreshError="1"/>
+      <sheetData sheetId="109" refreshError="1"/>
+      <sheetData sheetId="110" refreshError="1"/>
+      <sheetData sheetId="111" refreshError="1"/>
+      <sheetData sheetId="112" refreshError="1"/>
+      <sheetData sheetId="113" refreshError="1"/>
+      <sheetData sheetId="114" refreshError="1"/>
+      <sheetData sheetId="115" refreshError="1"/>
+      <sheetData sheetId="116" refreshError="1"/>
+      <sheetData sheetId="117" refreshError="1"/>
+      <sheetData sheetId="118" refreshError="1"/>
+      <sheetData sheetId="119" refreshError="1"/>
+      <sheetData sheetId="120" refreshError="1"/>
+      <sheetData sheetId="121" refreshError="1"/>
+      <sheetData sheetId="122" refreshError="1"/>
+      <sheetData sheetId="123" refreshError="1"/>
+      <sheetData sheetId="124" refreshError="1"/>
+      <sheetData sheetId="125" refreshError="1"/>
+      <sheetData sheetId="126" refreshError="1"/>
+      <sheetData sheetId="127" refreshError="1"/>
+      <sheetData sheetId="128" refreshError="1"/>
+      <sheetData sheetId="129" refreshError="1"/>
+      <sheetData sheetId="130" refreshError="1"/>
+      <sheetData sheetId="131">
+        <row r="2">
+          <cell r="N2">
+            <v>9.0687098494115101</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="N3">
+            <v>1</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="132">
+        <row r="2">
+          <cell r="N2">
+            <v>1.5833945082514056</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="N3">
+            <v>2</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="133" refreshError="1"/>
+      <sheetData sheetId="134">
+        <row r="2">
+          <cell r="N2">
+            <v>0.34825628167808953</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="N3">
+            <v>2</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="135" refreshError="1"/>
+      <sheetData sheetId="136">
+        <row r="2">
+          <cell r="N2">
+            <v>0.34825628167808953</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="B5" t="str">
+            <v>Spacer 2</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="137" refreshError="1"/>
+      <sheetData sheetId="138" refreshError="1"/>
+      <sheetData sheetId="139" refreshError="1"/>
+      <sheetData sheetId="140" refreshError="1"/>
+      <sheetData sheetId="141" refreshError="1"/>
+      <sheetData sheetId="142" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
@@ -3835,7 +4900,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3870,7 +4935,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4081,8 +5146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17448,7 +18513,7 @@
   <dimension ref="A2:N24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18132,9 +19197,7 @@
   </sheetPr>
   <dimension ref="A2:N24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -18736,6 +19799,3018 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="9" tint="-0.499984740745262"/>
+  </sheetPr>
+  <dimension ref="A1:O47"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="69.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" s="309"/>
+      <c r="B1" s="310"/>
+      <c r="C1" s="310"/>
+      <c r="D1" s="310"/>
+      <c r="E1" s="310"/>
+      <c r="F1" s="310"/>
+      <c r="G1" s="310"/>
+      <c r="H1" s="310"/>
+      <c r="I1" s="310"/>
+      <c r="J1" s="310"/>
+      <c r="K1" s="310"/>
+      <c r="L1" s="310"/>
+      <c r="M1" s="310"/>
+      <c r="N1" s="310"/>
+      <c r="O1" s="311"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" s="312" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="293" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="168" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="101">
+        <v>81</v>
+      </c>
+      <c r="L2" s="88"/>
+      <c r="M2" s="167" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" s="107">
+        <f>E14+I38+J46</f>
+        <v>18.300321314767661</v>
+      </c>
+      <c r="O2" s="313"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" s="312" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="88"/>
+      <c r="D3" s="167" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="293"/>
+      <c r="F3" s="88"/>
+      <c r="G3" s="88"/>
+      <c r="H3" s="88"/>
+      <c r="I3" s="88"/>
+      <c r="J3" s="88"/>
+      <c r="K3" s="88"/>
+      <c r="L3" s="88"/>
+      <c r="M3" s="167" t="s">
+        <v>7</v>
+      </c>
+      <c r="N3" s="103">
+        <v>2</v>
+      </c>
+      <c r="O3" s="313"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" s="312" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="C4" s="88"/>
+      <c r="D4" s="167" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="88"/>
+      <c r="F4" s="88"/>
+      <c r="G4" s="88"/>
+      <c r="H4" s="88"/>
+      <c r="I4" s="88"/>
+      <c r="J4" s="169" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" s="88"/>
+      <c r="L4" s="88"/>
+      <c r="M4" s="88"/>
+      <c r="N4" s="88"/>
+      <c r="O4" s="313"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" s="312" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>352</v>
+      </c>
+      <c r="C5" s="88"/>
+      <c r="D5" s="167" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="88"/>
+      <c r="F5" s="88"/>
+      <c r="G5" s="88"/>
+      <c r="H5" s="88"/>
+      <c r="I5" s="88"/>
+      <c r="J5" s="169" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" s="88"/>
+      <c r="L5" s="88"/>
+      <c r="M5" s="167" t="s">
+        <v>13</v>
+      </c>
+      <c r="N5" s="107">
+        <f>N3*N2</f>
+        <v>36.600642629535322</v>
+      </c>
+      <c r="O5" s="313"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" s="312" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="88"/>
+      <c r="D6" s="88"/>
+      <c r="E6" s="88"/>
+      <c r="F6" s="88"/>
+      <c r="G6" s="88"/>
+      <c r="H6" s="88"/>
+      <c r="I6" s="88"/>
+      <c r="J6" s="169" t="s">
+        <v>16</v>
+      </c>
+      <c r="K6" s="88"/>
+      <c r="L6" s="88"/>
+      <c r="M6" s="88"/>
+      <c r="N6" s="88"/>
+      <c r="O6" s="313"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7" s="312" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="100" t="s">
+        <v>354</v>
+      </c>
+      <c r="C7" s="88"/>
+      <c r="D7" s="88"/>
+      <c r="E7" s="88"/>
+      <c r="F7" s="88"/>
+      <c r="G7" s="88"/>
+      <c r="H7" s="88"/>
+      <c r="I7" s="88"/>
+      <c r="J7" s="88"/>
+      <c r="K7" s="88"/>
+      <c r="L7" s="88"/>
+      <c r="M7" s="88"/>
+      <c r="N7" s="88"/>
+      <c r="O7" s="313"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8" s="314"/>
+      <c r="B8" s="110"/>
+      <c r="C8" s="110"/>
+      <c r="D8" s="110"/>
+      <c r="E8" s="110"/>
+      <c r="F8" s="88"/>
+      <c r="G8" s="88"/>
+      <c r="H8" s="88"/>
+      <c r="I8" s="88"/>
+      <c r="J8" s="88"/>
+      <c r="K8" s="88"/>
+      <c r="L8" s="88"/>
+      <c r="M8" s="88"/>
+      <c r="N8" s="88"/>
+      <c r="O8" s="313"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" s="315" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="78" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="78" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="78" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="78" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="313"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" s="130">
+        <v>10</v>
+      </c>
+      <c r="B10" s="45" t="str">
+        <f>'ST 05001'!B5</f>
+        <v>Steering rod tube</v>
+      </c>
+      <c r="C10" s="131">
+        <f>'[2]SU 12001'!N2</f>
+        <v>9.0687098494115101</v>
+      </c>
+      <c r="D10" s="348">
+        <f>SU_12001_q</f>
+        <v>1</v>
+      </c>
+      <c r="E10" s="131">
+        <f>C10*D10</f>
+        <v>9.0687098494115101</v>
+      </c>
+      <c r="F10" s="88"/>
+      <c r="G10" s="88"/>
+      <c r="H10" s="88"/>
+      <c r="I10" s="88"/>
+      <c r="J10" s="88"/>
+      <c r="K10" s="88"/>
+      <c r="L10" s="88"/>
+      <c r="M10" s="88"/>
+      <c r="N10" s="88"/>
+      <c r="O10" s="313"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11" s="130">
+        <v>20</v>
+      </c>
+      <c r="B11" s="45" t="str">
+        <f>'ST 05002'!B5</f>
+        <v>Steering rod insert</v>
+      </c>
+      <c r="C11" s="131">
+        <f>'[2]SU 12002'!N2</f>
+        <v>1.5833945082514056</v>
+      </c>
+      <c r="D11" s="348">
+        <f>SU_12002_q</f>
+        <v>2</v>
+      </c>
+      <c r="E11" s="131">
+        <f t="shared" ref="E11:E13" si="0">C11*D11</f>
+        <v>3.1667890165028112</v>
+      </c>
+      <c r="F11" s="88"/>
+      <c r="G11" s="88"/>
+      <c r="H11" s="88"/>
+      <c r="I11" s="88"/>
+      <c r="J11" s="88"/>
+      <c r="K11" s="88"/>
+      <c r="L11" s="88"/>
+      <c r="M11" s="88"/>
+      <c r="N11" s="88"/>
+      <c r="O11" s="313"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12" s="130">
+        <v>30</v>
+      </c>
+      <c r="B12" s="45" t="str">
+        <f>'ST 05003'!B5</f>
+        <v>Spacer</v>
+      </c>
+      <c r="C12" s="131">
+        <f>'[2]SU 12003'!N2</f>
+        <v>0.34825628167808953</v>
+      </c>
+      <c r="D12" s="348">
+        <f>SU_12003_q</f>
+        <v>2</v>
+      </c>
+      <c r="E12" s="131">
+        <f t="shared" si="0"/>
+        <v>0.69651256335617906</v>
+      </c>
+      <c r="F12" s="88"/>
+      <c r="G12" s="88"/>
+      <c r="H12" s="88"/>
+      <c r="I12" s="88"/>
+      <c r="J12" s="88"/>
+      <c r="K12" s="88"/>
+      <c r="L12" s="88"/>
+      <c r="M12" s="88"/>
+      <c r="N12" s="88"/>
+      <c r="O12" s="313"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13" s="130">
+        <v>30</v>
+      </c>
+      <c r="B13" s="45" t="str">
+        <f>'[2]SU 12004'!B5</f>
+        <v>Spacer 2</v>
+      </c>
+      <c r="C13" s="131">
+        <f>'[2]SU 12004'!N2</f>
+        <v>0.34825628167808953</v>
+      </c>
+      <c r="D13" s="348">
+        <f>SU_12003_q</f>
+        <v>2</v>
+      </c>
+      <c r="E13" s="131">
+        <f t="shared" si="0"/>
+        <v>0.69651256335617906</v>
+      </c>
+      <c r="F13" s="104"/>
+      <c r="G13" s="104"/>
+      <c r="H13" s="104"/>
+      <c r="I13" s="104"/>
+      <c r="J13" s="104"/>
+      <c r="K13" s="104"/>
+      <c r="L13" s="104"/>
+      <c r="M13" s="104"/>
+      <c r="N13" s="104"/>
+      <c r="O13" s="316"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14" s="317"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="76" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="77">
+        <f>SUM(E10:E13)</f>
+        <v>13.628523992626681</v>
+      </c>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="313"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15" s="317"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="306"/>
+      <c r="D15" s="307"/>
+      <c r="E15" s="308"/>
+      <c r="F15" s="306"/>
+      <c r="G15" s="306"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="313"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16" s="315" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="78" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="78" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="78" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" s="78" t="s">
+        <v>31</v>
+      </c>
+      <c r="F16" s="78" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16" s="78" t="s">
+        <v>33</v>
+      </c>
+      <c r="H16" s="78" t="s">
+        <v>34</v>
+      </c>
+      <c r="I16" s="78" t="s">
+        <v>35</v>
+      </c>
+      <c r="J16" s="78" t="s">
+        <v>36</v>
+      </c>
+      <c r="K16" s="78" t="s">
+        <v>37</v>
+      </c>
+      <c r="L16" s="78" t="s">
+        <v>38</v>
+      </c>
+      <c r="M16" s="78" t="s">
+        <v>22</v>
+      </c>
+      <c r="N16" s="78" t="s">
+        <v>23</v>
+      </c>
+      <c r="O16" s="313"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A17" s="318">
+        <v>10</v>
+      </c>
+      <c r="B17" s="297" t="s">
+        <v>357</v>
+      </c>
+      <c r="C17" s="297" t="s">
+        <v>358</v>
+      </c>
+      <c r="D17" s="298">
+        <f>0.02*E17^2+1.22</f>
+        <v>1.94</v>
+      </c>
+      <c r="E17" s="297">
+        <v>6</v>
+      </c>
+      <c r="F17" s="297" t="s">
+        <v>62</v>
+      </c>
+      <c r="G17" s="297"/>
+      <c r="H17" s="299"/>
+      <c r="I17" s="300" t="s">
+        <v>359</v>
+      </c>
+      <c r="J17" s="301"/>
+      <c r="K17" s="299"/>
+      <c r="L17" s="299"/>
+      <c r="M17" s="301">
+        <v>1</v>
+      </c>
+      <c r="N17" s="54">
+        <f>D17*M17</f>
+        <v>1.94</v>
+      </c>
+      <c r="O17" s="313"/>
+    </row>
+    <row r="18" spans="1:15" s="304" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="318">
+        <v>20</v>
+      </c>
+      <c r="B18" s="297" t="s">
+        <v>357</v>
+      </c>
+      <c r="C18" s="297" t="s">
+        <v>360</v>
+      </c>
+      <c r="D18" s="298">
+        <f>0.02*E18^2+1.22</f>
+        <v>1.94</v>
+      </c>
+      <c r="E18" s="297">
+        <v>6</v>
+      </c>
+      <c r="F18" s="297" t="s">
+        <v>62</v>
+      </c>
+      <c r="G18" s="297"/>
+      <c r="H18" s="299"/>
+      <c r="I18" s="302" t="s">
+        <v>359</v>
+      </c>
+      <c r="J18" s="301"/>
+      <c r="K18" s="299"/>
+      <c r="L18" s="303"/>
+      <c r="M18" s="301">
+        <v>1</v>
+      </c>
+      <c r="N18" s="54">
+        <f>D18*M18</f>
+        <v>1.94</v>
+      </c>
+      <c r="O18" s="319"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A19" s="314"/>
+      <c r="B19" s="305"/>
+      <c r="C19" s="110"/>
+      <c r="D19" s="110"/>
+      <c r="E19" s="110"/>
+      <c r="F19" s="110"/>
+      <c r="G19" s="110"/>
+      <c r="H19" s="110"/>
+      <c r="I19" s="110"/>
+      <c r="J19" s="110"/>
+      <c r="K19" s="110"/>
+      <c r="L19" s="110"/>
+      <c r="M19" s="78" t="s">
+        <v>23</v>
+      </c>
+      <c r="N19" s="78">
+        <f>SUM(N17:N18)</f>
+        <v>3.88</v>
+      </c>
+      <c r="O19" s="313"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A20" s="317"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="313"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A21" s="315" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="78" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="78" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" s="78" t="s">
+        <v>30</v>
+      </c>
+      <c r="E21" s="78" t="s">
+        <v>43</v>
+      </c>
+      <c r="F21" s="78" t="s">
+        <v>22</v>
+      </c>
+      <c r="G21" s="78" t="s">
+        <v>44</v>
+      </c>
+      <c r="H21" s="78" t="s">
+        <v>45</v>
+      </c>
+      <c r="I21" s="78" t="s">
+        <v>23</v>
+      </c>
+      <c r="J21" s="41"/>
+      <c r="K21" s="41"/>
+      <c r="L21" s="41"/>
+      <c r="M21" s="41"/>
+      <c r="N21" s="41"/>
+      <c r="O21" s="313"/>
+    </row>
+    <row r="22" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="296">
+        <v>10</v>
+      </c>
+      <c r="B22" s="32" t="s">
+        <v>361</v>
+      </c>
+      <c r="C22" s="327" t="s">
+        <v>362</v>
+      </c>
+      <c r="D22" s="34">
+        <v>0.02</v>
+      </c>
+      <c r="E22" s="327" t="s">
+        <v>363</v>
+      </c>
+      <c r="F22" s="328">
+        <v>6.6</v>
+      </c>
+      <c r="G22" s="329"/>
+      <c r="H22" s="328">
+        <v>1</v>
+      </c>
+      <c r="I22" s="34">
+        <f>D22*F22*H22</f>
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="J22" s="88"/>
+      <c r="K22" s="88"/>
+      <c r="L22" s="88"/>
+      <c r="M22" s="88"/>
+      <c r="N22" s="88"/>
+      <c r="O22" s="295"/>
+    </row>
+    <row r="23" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="296">
+        <f>A22+10</f>
+        <v>20</v>
+      </c>
+      <c r="B23" s="32" t="s">
+        <v>361</v>
+      </c>
+      <c r="C23" s="327" t="s">
+        <v>364</v>
+      </c>
+      <c r="D23" s="34">
+        <v>0.02</v>
+      </c>
+      <c r="E23" s="327" t="s">
+        <v>363</v>
+      </c>
+      <c r="F23" s="328">
+        <v>6.6</v>
+      </c>
+      <c r="G23" s="328"/>
+      <c r="H23" s="328">
+        <v>1</v>
+      </c>
+      <c r="I23" s="34">
+        <f t="shared" ref="I23:I37" si="1">D23*F23*H23</f>
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="J23" s="88"/>
+      <c r="K23" s="88"/>
+      <c r="L23" s="88"/>
+      <c r="M23" s="88"/>
+      <c r="N23" s="88"/>
+      <c r="O23" s="295"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A24" s="296">
+        <f t="shared" ref="A24:A37" si="2">A23+10</f>
+        <v>30</v>
+      </c>
+      <c r="B24" s="330" t="s">
+        <v>365</v>
+      </c>
+      <c r="C24" s="331" t="s">
+        <v>366</v>
+      </c>
+      <c r="D24" s="107">
+        <v>0.02</v>
+      </c>
+      <c r="E24" s="331" t="s">
+        <v>150</v>
+      </c>
+      <c r="F24" s="328">
+        <v>6.6</v>
+      </c>
+      <c r="G24" s="331"/>
+      <c r="H24" s="331">
+        <v>1</v>
+      </c>
+      <c r="I24" s="34">
+        <f t="shared" si="1"/>
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="J24" s="88"/>
+      <c r="K24" s="88"/>
+      <c r="L24" s="88"/>
+      <c r="M24" s="88"/>
+      <c r="N24" s="88"/>
+      <c r="O24" s="295"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A25" s="296">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="B25" s="332" t="s">
+        <v>367</v>
+      </c>
+      <c r="C25" s="333" t="s">
+        <v>368</v>
+      </c>
+      <c r="D25" s="107">
+        <v>0.12</v>
+      </c>
+      <c r="E25" s="296" t="s">
+        <v>129</v>
+      </c>
+      <c r="F25" s="296">
+        <v>1</v>
+      </c>
+      <c r="G25" s="296"/>
+      <c r="H25" s="296">
+        <v>1</v>
+      </c>
+      <c r="I25" s="34">
+        <f t="shared" si="1"/>
+        <v>0.12</v>
+      </c>
+      <c r="J25" s="88"/>
+      <c r="K25" s="88"/>
+      <c r="L25" s="88"/>
+      <c r="M25" s="88"/>
+      <c r="N25" s="88"/>
+      <c r="O25" s="295"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A26" s="296">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="B26" s="332" t="s">
+        <v>369</v>
+      </c>
+      <c r="C26" s="333" t="s">
+        <v>370</v>
+      </c>
+      <c r="D26" s="107">
+        <v>0.5</v>
+      </c>
+      <c r="E26" s="334" t="s">
+        <v>129</v>
+      </c>
+      <c r="F26" s="296">
+        <v>1</v>
+      </c>
+      <c r="G26" s="296"/>
+      <c r="H26" s="296">
+        <v>1</v>
+      </c>
+      <c r="I26" s="34">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="J26" s="88"/>
+      <c r="K26" s="88"/>
+      <c r="L26" s="88"/>
+      <c r="M26" s="88"/>
+      <c r="N26" s="88"/>
+      <c r="O26" s="295"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A27" s="296">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="B27" s="332" t="s">
+        <v>158</v>
+      </c>
+      <c r="C27" s="333" t="s">
+        <v>371</v>
+      </c>
+      <c r="D27" s="107">
+        <v>1.5</v>
+      </c>
+      <c r="E27" s="296" t="s">
+        <v>129</v>
+      </c>
+      <c r="F27" s="296">
+        <v>1</v>
+      </c>
+      <c r="G27" s="296"/>
+      <c r="H27" s="296">
+        <v>1</v>
+      </c>
+      <c r="I27" s="34">
+        <f t="shared" si="1"/>
+        <v>1.5</v>
+      </c>
+      <c r="J27" s="88"/>
+      <c r="K27" s="88"/>
+      <c r="L27" s="88"/>
+      <c r="M27" s="88"/>
+      <c r="N27" s="88"/>
+      <c r="O27" s="295"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A28" s="296">
+        <f t="shared" si="2"/>
+        <v>70</v>
+      </c>
+      <c r="B28" s="332" t="s">
+        <v>372</v>
+      </c>
+      <c r="C28" s="333" t="s">
+        <v>371</v>
+      </c>
+      <c r="D28" s="107">
+        <v>0.25</v>
+      </c>
+      <c r="E28" s="296" t="s">
+        <v>129</v>
+      </c>
+      <c r="F28" s="296">
+        <v>1</v>
+      </c>
+      <c r="G28" s="296"/>
+      <c r="H28" s="296">
+        <v>1</v>
+      </c>
+      <c r="I28" s="34">
+        <f t="shared" si="1"/>
+        <v>0.25</v>
+      </c>
+      <c r="J28" s="88"/>
+      <c r="K28" s="88"/>
+      <c r="L28" s="88"/>
+      <c r="M28" s="88"/>
+      <c r="N28" s="88"/>
+      <c r="O28" s="295"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A29" s="296">
+        <f t="shared" si="2"/>
+        <v>80</v>
+      </c>
+      <c r="B29" s="333" t="s">
+        <v>373</v>
+      </c>
+      <c r="C29" s="333" t="s">
+        <v>374</v>
+      </c>
+      <c r="D29" s="335">
+        <v>0.06</v>
+      </c>
+      <c r="E29" s="336" t="s">
+        <v>129</v>
+      </c>
+      <c r="F29" s="336">
+        <v>1</v>
+      </c>
+      <c r="G29" s="336"/>
+      <c r="H29" s="336">
+        <v>1</v>
+      </c>
+      <c r="I29" s="34">
+        <f t="shared" si="1"/>
+        <v>0.06</v>
+      </c>
+      <c r="J29" s="88"/>
+      <c r="K29" s="88"/>
+      <c r="L29" s="88"/>
+      <c r="M29" s="88"/>
+      <c r="N29" s="88"/>
+      <c r="O29" s="295"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A30" s="296">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+      <c r="B30" s="333" t="s">
+        <v>373</v>
+      </c>
+      <c r="C30" s="333" t="s">
+        <v>375</v>
+      </c>
+      <c r="D30" s="335">
+        <v>0.06</v>
+      </c>
+      <c r="E30" s="336" t="s">
+        <v>129</v>
+      </c>
+      <c r="F30" s="336">
+        <v>1</v>
+      </c>
+      <c r="G30" s="336"/>
+      <c r="H30" s="336">
+        <v>1</v>
+      </c>
+      <c r="I30" s="34">
+        <f t="shared" si="1"/>
+        <v>0.06</v>
+      </c>
+      <c r="J30" s="88"/>
+      <c r="K30" s="88"/>
+      <c r="L30" s="88"/>
+      <c r="M30" s="88"/>
+      <c r="N30" s="88"/>
+      <c r="O30" s="295"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A31" s="296">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="B31" s="332" t="s">
+        <v>367</v>
+      </c>
+      <c r="C31" s="333" t="s">
+        <v>376</v>
+      </c>
+      <c r="D31" s="335">
+        <v>0.12</v>
+      </c>
+      <c r="E31" s="336" t="s">
+        <v>129</v>
+      </c>
+      <c r="F31" s="336">
+        <v>1</v>
+      </c>
+      <c r="G31" s="336"/>
+      <c r="H31" s="336">
+        <v>1</v>
+      </c>
+      <c r="I31" s="34">
+        <f t="shared" si="1"/>
+        <v>0.12</v>
+      </c>
+      <c r="J31" s="88"/>
+      <c r="K31" s="88"/>
+      <c r="L31" s="88"/>
+      <c r="M31" s="88"/>
+      <c r="N31" s="88"/>
+      <c r="O31" s="295"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A32" s="296">
+        <f t="shared" si="2"/>
+        <v>110</v>
+      </c>
+      <c r="B32" s="336" t="s">
+        <v>373</v>
+      </c>
+      <c r="C32" s="333" t="s">
+        <v>377</v>
+      </c>
+      <c r="D32" s="335">
+        <v>0.06</v>
+      </c>
+      <c r="E32" s="336" t="s">
+        <v>129</v>
+      </c>
+      <c r="F32" s="336">
+        <v>1</v>
+      </c>
+      <c r="G32" s="336"/>
+      <c r="H32" s="336">
+        <v>1</v>
+      </c>
+      <c r="I32" s="34">
+        <f t="shared" si="1"/>
+        <v>0.06</v>
+      </c>
+      <c r="J32" s="88"/>
+      <c r="K32" s="88"/>
+      <c r="L32" s="88"/>
+      <c r="M32" s="88"/>
+      <c r="N32" s="88"/>
+      <c r="O32" s="295"/>
+    </row>
+    <row r="33" spans="1:15" s="338" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="296">
+        <f t="shared" si="2"/>
+        <v>120</v>
+      </c>
+      <c r="B33" s="336" t="s">
+        <v>373</v>
+      </c>
+      <c r="C33" s="333" t="s">
+        <v>378</v>
+      </c>
+      <c r="D33" s="335">
+        <v>0.06</v>
+      </c>
+      <c r="E33" s="336" t="s">
+        <v>129</v>
+      </c>
+      <c r="F33" s="336">
+        <v>1</v>
+      </c>
+      <c r="G33" s="336"/>
+      <c r="H33" s="336">
+        <v>1</v>
+      </c>
+      <c r="I33" s="34">
+        <f t="shared" si="1"/>
+        <v>0.06</v>
+      </c>
+      <c r="J33" s="104"/>
+      <c r="K33" s="104"/>
+      <c r="L33" s="104"/>
+      <c r="M33" s="104"/>
+      <c r="N33" s="104"/>
+      <c r="O33" s="337"/>
+    </row>
+    <row r="34" spans="1:15" s="340" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="296">
+        <f t="shared" si="2"/>
+        <v>130</v>
+      </c>
+      <c r="B34" s="332" t="s">
+        <v>367</v>
+      </c>
+      <c r="C34" s="333" t="s">
+        <v>379</v>
+      </c>
+      <c r="D34" s="335">
+        <v>0.12</v>
+      </c>
+      <c r="E34" s="336" t="s">
+        <v>129</v>
+      </c>
+      <c r="F34" s="336">
+        <v>1</v>
+      </c>
+      <c r="G34" s="336"/>
+      <c r="H34" s="336">
+        <v>1</v>
+      </c>
+      <c r="I34" s="34">
+        <f t="shared" si="1"/>
+        <v>0.12</v>
+      </c>
+      <c r="J34" s="104"/>
+      <c r="K34" s="104"/>
+      <c r="L34" s="104"/>
+      <c r="M34" s="104"/>
+      <c r="N34" s="104"/>
+      <c r="O34" s="339"/>
+    </row>
+    <row r="35" spans="1:15" s="340" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="296">
+        <f t="shared" si="2"/>
+        <v>140</v>
+      </c>
+      <c r="B35" s="332" t="s">
+        <v>367</v>
+      </c>
+      <c r="C35" s="333" t="s">
+        <v>380</v>
+      </c>
+      <c r="D35" s="335">
+        <v>0.12</v>
+      </c>
+      <c r="E35" s="336" t="s">
+        <v>129</v>
+      </c>
+      <c r="F35" s="336">
+        <v>1</v>
+      </c>
+      <c r="G35" s="336"/>
+      <c r="H35" s="336">
+        <v>1</v>
+      </c>
+      <c r="I35" s="34">
+        <f t="shared" si="1"/>
+        <v>0.12</v>
+      </c>
+      <c r="J35" s="104"/>
+      <c r="K35" s="104"/>
+      <c r="L35" s="104"/>
+      <c r="M35" s="104"/>
+      <c r="N35" s="104"/>
+      <c r="O35" s="339"/>
+    </row>
+    <row r="36" spans="1:15" s="338" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="296">
+        <f t="shared" si="2"/>
+        <v>150</v>
+      </c>
+      <c r="B36" s="332" t="s">
+        <v>145</v>
+      </c>
+      <c r="C36" s="333" t="s">
+        <v>371</v>
+      </c>
+      <c r="D36" s="335">
+        <v>0.75</v>
+      </c>
+      <c r="E36" s="336" t="s">
+        <v>129</v>
+      </c>
+      <c r="F36" s="336">
+        <v>1</v>
+      </c>
+      <c r="G36" s="336"/>
+      <c r="H36" s="336">
+        <v>1</v>
+      </c>
+      <c r="I36" s="34">
+        <f t="shared" si="1"/>
+        <v>0.75</v>
+      </c>
+      <c r="J36" s="104"/>
+      <c r="K36" s="104"/>
+      <c r="L36" s="104"/>
+      <c r="M36" s="104"/>
+      <c r="N36" s="104"/>
+      <c r="O36" s="337"/>
+    </row>
+    <row r="37" spans="1:15" s="338" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="296">
+        <f t="shared" si="2"/>
+        <v>160</v>
+      </c>
+      <c r="B37" s="332" t="s">
+        <v>372</v>
+      </c>
+      <c r="C37" s="333" t="s">
+        <v>371</v>
+      </c>
+      <c r="D37" s="335">
+        <v>0.25</v>
+      </c>
+      <c r="E37" s="336" t="s">
+        <v>129</v>
+      </c>
+      <c r="F37" s="336">
+        <v>1</v>
+      </c>
+      <c r="G37" s="336"/>
+      <c r="H37" s="336">
+        <v>1</v>
+      </c>
+      <c r="I37" s="34">
+        <f t="shared" si="1"/>
+        <v>0.25</v>
+      </c>
+      <c r="J37" s="104"/>
+      <c r="K37" s="104"/>
+      <c r="L37" s="104"/>
+      <c r="M37" s="104"/>
+      <c r="N37" s="104"/>
+      <c r="O37" s="337"/>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A38" s="320"/>
+      <c r="B38" s="41"/>
+      <c r="C38" s="41"/>
+      <c r="D38" s="41"/>
+      <c r="E38" s="41"/>
+      <c r="F38" s="41"/>
+      <c r="G38" s="41"/>
+      <c r="H38" s="76" t="s">
+        <v>23</v>
+      </c>
+      <c r="I38" s="77">
+        <f>SUM(I22:I37)</f>
+        <v>4.3660000000000005</v>
+      </c>
+      <c r="J38" s="41"/>
+      <c r="K38" s="41"/>
+      <c r="L38" s="162"/>
+      <c r="M38" s="41"/>
+      <c r="N38" s="41"/>
+      <c r="O38" s="313"/>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A39" s="317"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1"/>
+      <c r="L39" s="1"/>
+      <c r="M39" s="1"/>
+      <c r="N39" s="1"/>
+      <c r="O39" s="313"/>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A40" s="315" t="s">
+        <v>19</v>
+      </c>
+      <c r="B40" s="78" t="s">
+        <v>63</v>
+      </c>
+      <c r="C40" s="78" t="s">
+        <v>29</v>
+      </c>
+      <c r="D40" s="78" t="s">
+        <v>30</v>
+      </c>
+      <c r="E40" s="78" t="s">
+        <v>31</v>
+      </c>
+      <c r="F40" s="78" t="s">
+        <v>32</v>
+      </c>
+      <c r="G40" s="78" t="s">
+        <v>33</v>
+      </c>
+      <c r="H40" s="78" t="s">
+        <v>34</v>
+      </c>
+      <c r="I40" s="78" t="s">
+        <v>22</v>
+      </c>
+      <c r="J40" s="78" t="s">
+        <v>23</v>
+      </c>
+      <c r="K40" s="41"/>
+      <c r="L40" s="41"/>
+      <c r="M40" s="41"/>
+      <c r="N40" s="41"/>
+      <c r="O40" s="313"/>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A41" s="296">
+        <v>10</v>
+      </c>
+      <c r="B41" s="296" t="s">
+        <v>381</v>
+      </c>
+      <c r="C41" s="296" t="s">
+        <v>382</v>
+      </c>
+      <c r="D41" s="341">
+        <f>0.8/105154*E41^2*G41*SQRT(G41)+0.003*EXP(0.319*E41)</f>
+        <v>0.10301760876586051</v>
+      </c>
+      <c r="E41" s="342">
+        <v>6</v>
+      </c>
+      <c r="F41" s="342" t="s">
+        <v>62</v>
+      </c>
+      <c r="G41" s="342">
+        <v>45</v>
+      </c>
+      <c r="H41" s="342" t="s">
+        <v>62</v>
+      </c>
+      <c r="I41" s="103">
+        <v>1</v>
+      </c>
+      <c r="J41" s="107">
+        <f>D41*I41</f>
+        <v>0.10301760876586051</v>
+      </c>
+      <c r="K41" s="88"/>
+      <c r="L41" s="88"/>
+      <c r="M41" s="88"/>
+      <c r="N41" s="88"/>
+      <c r="O41" s="295"/>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A42" s="296">
+        <f>A41+10</f>
+        <v>20</v>
+      </c>
+      <c r="B42" s="296" t="s">
+        <v>381</v>
+      </c>
+      <c r="C42" s="296" t="s">
+        <v>383</v>
+      </c>
+      <c r="D42" s="341">
+        <f>0.8/105154*E42^2*G42*SQRT(G42)+0.003*EXP(0.319*E42)</f>
+        <v>0.10301760876586051</v>
+      </c>
+      <c r="E42" s="342">
+        <v>6</v>
+      </c>
+      <c r="F42" s="342" t="s">
+        <v>62</v>
+      </c>
+      <c r="G42" s="342">
+        <v>45</v>
+      </c>
+      <c r="H42" s="342" t="s">
+        <v>62</v>
+      </c>
+      <c r="I42" s="103">
+        <v>1</v>
+      </c>
+      <c r="J42" s="107">
+        <f t="shared" ref="J42:J45" si="3">D42*I42</f>
+        <v>0.10301760876586051</v>
+      </c>
+      <c r="K42" s="88"/>
+      <c r="L42" s="88"/>
+      <c r="M42" s="88"/>
+      <c r="N42" s="88"/>
+      <c r="O42" s="295"/>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A43" s="296">
+        <f t="shared" ref="A43:A45" si="4">A42+10</f>
+        <v>30</v>
+      </c>
+      <c r="B43" s="296" t="s">
+        <v>130</v>
+      </c>
+      <c r="C43" s="296"/>
+      <c r="D43" s="341">
+        <v>0.01</v>
+      </c>
+      <c r="E43" s="296">
+        <v>6</v>
+      </c>
+      <c r="F43" s="343" t="s">
+        <v>129</v>
+      </c>
+      <c r="G43" s="296"/>
+      <c r="H43" s="296"/>
+      <c r="I43" s="103">
+        <v>4</v>
+      </c>
+      <c r="J43" s="107">
+        <f t="shared" si="3"/>
+        <v>0.04</v>
+      </c>
+      <c r="K43" s="88"/>
+      <c r="L43" s="88"/>
+      <c r="M43" s="88"/>
+      <c r="N43" s="88"/>
+      <c r="O43" s="295"/>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A44" s="296">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+      <c r="B44" s="296" t="s">
+        <v>132</v>
+      </c>
+      <c r="C44" s="296" t="s">
+        <v>384</v>
+      </c>
+      <c r="D44" s="341">
+        <f>0.009*EXP(0.2*E44)</f>
+        <v>2.9881052304628931E-2</v>
+      </c>
+      <c r="E44" s="296">
+        <v>6</v>
+      </c>
+      <c r="F44" s="343" t="s">
+        <v>62</v>
+      </c>
+      <c r="G44" s="296"/>
+      <c r="H44" s="296"/>
+      <c r="I44" s="103">
+        <v>1</v>
+      </c>
+      <c r="J44" s="107">
+        <f t="shared" si="3"/>
+        <v>2.9881052304628931E-2</v>
+      </c>
+      <c r="K44" s="88"/>
+      <c r="L44" s="88"/>
+      <c r="M44" s="88"/>
+      <c r="N44" s="88"/>
+      <c r="O44" s="295"/>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A45" s="296">
+        <f t="shared" si="4"/>
+        <v>50</v>
+      </c>
+      <c r="B45" s="296" t="s">
+        <v>132</v>
+      </c>
+      <c r="C45" s="296" t="s">
+        <v>385</v>
+      </c>
+      <c r="D45" s="341">
+        <f>0.009*EXP(0.2*E45)</f>
+        <v>2.9881052304628931E-2</v>
+      </c>
+      <c r="E45" s="296">
+        <v>6</v>
+      </c>
+      <c r="F45" s="343" t="s">
+        <v>62</v>
+      </c>
+      <c r="G45" s="296"/>
+      <c r="H45" s="296"/>
+      <c r="I45" s="103">
+        <v>1</v>
+      </c>
+      <c r="J45" s="107">
+        <f t="shared" si="3"/>
+        <v>2.9881052304628931E-2</v>
+      </c>
+      <c r="K45" s="88"/>
+      <c r="L45" s="88"/>
+      <c r="M45" s="88"/>
+      <c r="N45" s="88"/>
+      <c r="O45" s="295"/>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A46" s="320"/>
+      <c r="B46" s="41"/>
+      <c r="C46" s="41"/>
+      <c r="D46" s="41"/>
+      <c r="E46" s="41"/>
+      <c r="F46" s="41"/>
+      <c r="G46" s="41"/>
+      <c r="H46" s="41"/>
+      <c r="I46" s="170" t="s">
+        <v>23</v>
+      </c>
+      <c r="J46" s="172">
+        <f>SUM(J41:J45)</f>
+        <v>0.30579732214097893</v>
+      </c>
+      <c r="K46" s="1"/>
+      <c r="L46" s="1"/>
+      <c r="M46" s="1"/>
+      <c r="N46" s="1"/>
+      <c r="O46" s="313"/>
+    </row>
+    <row r="47" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="321"/>
+      <c r="B47" s="322"/>
+      <c r="C47" s="322"/>
+      <c r="D47" s="322"/>
+      <c r="E47" s="322"/>
+      <c r="F47" s="322"/>
+      <c r="G47" s="322"/>
+      <c r="H47" s="323"/>
+      <c r="I47" s="324"/>
+      <c r="J47" s="322"/>
+      <c r="K47" s="325"/>
+      <c r="L47" s="325"/>
+      <c r="M47" s="325"/>
+      <c r="N47" s="325"/>
+      <c r="O47" s="326"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" location="BOM!A1" display="Back to BOM"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="9" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:O17"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.33203125" customWidth="1"/>
+    <col min="10" max="10" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" s="309"/>
+      <c r="B1" s="310"/>
+      <c r="C1" s="310"/>
+      <c r="D1" s="310"/>
+      <c r="E1" s="310"/>
+      <c r="F1" s="310"/>
+      <c r="G1" s="310"/>
+      <c r="H1" s="310"/>
+      <c r="I1" s="310"/>
+      <c r="J1" s="310"/>
+      <c r="K1" s="310"/>
+      <c r="L1" s="310"/>
+      <c r="M1" s="310"/>
+      <c r="N1" s="310"/>
+      <c r="O1" s="311"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" s="344" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="207" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="3">
+        <v>81</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="202" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" s="4">
+        <f>N12+I16</f>
+        <v>9.787952354709665</v>
+      </c>
+      <c r="O2" s="313"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" s="344" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="202" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="202" t="s">
+        <v>7</v>
+      </c>
+      <c r="N3" s="5">
+        <v>1</v>
+      </c>
+      <c r="O3" s="313"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" s="344" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="202" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="202" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="313"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" s="344" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="202" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="202" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="202" t="s">
+        <v>13</v>
+      </c>
+      <c r="N5" s="4">
+        <f>N2*N3</f>
+        <v>9.787952354709665</v>
+      </c>
+      <c r="O5" s="313"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" s="344" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="202" t="s">
+        <v>16</v>
+      </c>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="313"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7" s="344" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="313"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8" s="344" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="313"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" s="317"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="313"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" s="345" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="203" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="203" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="203" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="203" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="203" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="203" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" s="203" t="s">
+        <v>34</v>
+      </c>
+      <c r="I10" s="203" t="s">
+        <v>35</v>
+      </c>
+      <c r="J10" s="203" t="s">
+        <v>36</v>
+      </c>
+      <c r="K10" s="203" t="s">
+        <v>37</v>
+      </c>
+      <c r="L10" s="203" t="s">
+        <v>38</v>
+      </c>
+      <c r="M10" s="203" t="s">
+        <v>22</v>
+      </c>
+      <c r="N10" s="203" t="s">
+        <v>23</v>
+      </c>
+      <c r="O10" s="313"/>
+    </row>
+    <row r="11" spans="1:15" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="350">
+        <v>10</v>
+      </c>
+      <c r="B11" s="351" t="s">
+        <v>390</v>
+      </c>
+      <c r="C11" s="352" t="s">
+        <v>391</v>
+      </c>
+      <c r="D11" s="353">
+        <v>200</v>
+      </c>
+      <c r="E11" s="354">
+        <f>J11*K11*L11</f>
+        <v>4.3502010465376287E-2</v>
+      </c>
+      <c r="F11" s="355" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" s="355"/>
+      <c r="H11" s="356"/>
+      <c r="I11" s="349" t="s">
+        <v>392</v>
+      </c>
+      <c r="J11" s="357">
+        <f>PI()*((8*10^-3)^2-(6*10^-3)^2)</f>
+        <v>8.7964594300514196E-5</v>
+      </c>
+      <c r="K11" s="358">
+        <v>0.313</v>
+      </c>
+      <c r="L11" s="359">
+        <v>1580</v>
+      </c>
+      <c r="M11" s="359">
+        <v>1</v>
+      </c>
+      <c r="N11" s="353">
+        <f>D11*E11</f>
+        <v>8.7004020930752581</v>
+      </c>
+      <c r="O11" s="313"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12" s="320"/>
+      <c r="B12" s="41"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="41"/>
+      <c r="I12" s="41"/>
+      <c r="J12" s="41"/>
+      <c r="K12" s="41"/>
+      <c r="L12" s="41"/>
+      <c r="M12" s="198" t="s">
+        <v>23</v>
+      </c>
+      <c r="N12" s="199">
+        <f>SUM(N11)</f>
+        <v>8.7004020930752581</v>
+      </c>
+      <c r="O12" s="313"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13" s="317"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="313"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14" s="345" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="203" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="203" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="203" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="203" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="203" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" s="203" t="s">
+        <v>44</v>
+      </c>
+      <c r="H14" s="203" t="s">
+        <v>45</v>
+      </c>
+      <c r="I14" s="203" t="s">
+        <v>23</v>
+      </c>
+      <c r="J14" s="41"/>
+      <c r="K14" s="41"/>
+      <c r="L14" s="41"/>
+      <c r="M14" s="41"/>
+      <c r="N14" s="41"/>
+      <c r="O14" s="313"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15" s="360">
+        <v>10</v>
+      </c>
+      <c r="B15" s="361" t="s">
+        <v>393</v>
+      </c>
+      <c r="C15" s="362" t="s">
+        <v>394</v>
+      </c>
+      <c r="D15" s="363">
+        <v>25</v>
+      </c>
+      <c r="E15" s="361" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="364">
+        <f>E11</f>
+        <v>4.3502010465376287E-2</v>
+      </c>
+      <c r="G15" s="365"/>
+      <c r="H15" s="365"/>
+      <c r="I15" s="366">
+        <f>D15*F15</f>
+        <v>1.0875502616344073</v>
+      </c>
+      <c r="J15" s="367"/>
+      <c r="K15" s="367"/>
+      <c r="L15" s="367"/>
+      <c r="M15" s="367"/>
+      <c r="N15" s="367"/>
+      <c r="O15" s="313"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16" s="320"/>
+      <c r="B16" s="41"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="208" t="s">
+        <v>23</v>
+      </c>
+      <c r="I16" s="209">
+        <f>SUM(I15)</f>
+        <v>1.0875502616344073</v>
+      </c>
+      <c r="J16" s="41"/>
+      <c r="K16" s="41"/>
+      <c r="L16" s="41"/>
+      <c r="M16" s="41"/>
+      <c r="N16" s="41"/>
+      <c r="O16" s="313"/>
+    </row>
+    <row r="17" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="346"/>
+      <c r="B17" s="347"/>
+      <c r="C17" s="347"/>
+      <c r="D17" s="347"/>
+      <c r="E17" s="347"/>
+      <c r="F17" s="347"/>
+      <c r="G17" s="347"/>
+      <c r="H17" s="347"/>
+      <c r="I17" s="347"/>
+      <c r="J17" s="347"/>
+      <c r="K17" s="347"/>
+      <c r="L17" s="347"/>
+      <c r="M17" s="347"/>
+      <c r="N17" s="347"/>
+      <c r="O17" s="326"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" location="BOM!A1" display="Back to BOM"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="9" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:O21"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5546875" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.77734375" customWidth="1"/>
+    <col min="12" max="12" width="11.109375" customWidth="1"/>
+    <col min="13" max="13" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" s="309"/>
+      <c r="B1" s="310"/>
+      <c r="C1" s="310"/>
+      <c r="D1" s="310"/>
+      <c r="E1" s="310"/>
+      <c r="F1" s="310"/>
+      <c r="G1" s="310"/>
+      <c r="H1" s="310"/>
+      <c r="I1" s="310"/>
+      <c r="J1" s="310"/>
+      <c r="K1" s="310"/>
+      <c r="L1" s="310"/>
+      <c r="M1" s="310"/>
+      <c r="N1" s="310"/>
+      <c r="O1" s="311"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" s="344" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="207" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="3">
+        <v>81</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="202" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" s="4" t="e">
+        <f>N12+I20</f>
+        <v>#REF!</v>
+      </c>
+      <c r="O2" s="313"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" s="344" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="202" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="202" t="s">
+        <v>7</v>
+      </c>
+      <c r="N3" s="5">
+        <v>1</v>
+      </c>
+      <c r="O3" s="313"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" s="344" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="202" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="202" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="313"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" s="344" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>356</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="202" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="202" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="202" t="s">
+        <v>13</v>
+      </c>
+      <c r="N5" s="4" t="e">
+        <f>N2*N3</f>
+        <v>#REF!</v>
+      </c>
+      <c r="O5" s="313"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" s="344" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="202" t="s">
+        <v>16</v>
+      </c>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="313"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7" s="344" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="313"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8" s="344" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="313"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" s="317"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="313"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" s="345" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="203" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="203" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="203" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="203" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="203" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="203" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" s="203" t="s">
+        <v>34</v>
+      </c>
+      <c r="I10" s="203" t="s">
+        <v>35</v>
+      </c>
+      <c r="J10" s="203" t="s">
+        <v>36</v>
+      </c>
+      <c r="K10" s="203" t="s">
+        <v>37</v>
+      </c>
+      <c r="L10" s="203" t="s">
+        <v>38</v>
+      </c>
+      <c r="M10" s="203" t="s">
+        <v>22</v>
+      </c>
+      <c r="N10" s="203" t="s">
+        <v>23</v>
+      </c>
+      <c r="O10" s="313"/>
+    </row>
+    <row r="11" spans="1:15" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="374">
+        <v>10</v>
+      </c>
+      <c r="B11" s="375" t="s">
+        <v>395</v>
+      </c>
+      <c r="C11" s="374" t="s">
+        <v>396</v>
+      </c>
+      <c r="D11" s="376">
+        <v>4.2</v>
+      </c>
+      <c r="E11" s="377">
+        <f>J11*K11*L11</f>
+        <v>6.9915359107477454E-2</v>
+      </c>
+      <c r="F11" s="374" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" s="374"/>
+      <c r="H11" s="378"/>
+      <c r="I11" s="379" t="s">
+        <v>397</v>
+      </c>
+      <c r="J11" s="370">
+        <f>PI()*9*9/1000000</f>
+        <v>2.5446900494077322E-4</v>
+      </c>
+      <c r="K11" s="371">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="L11" s="369">
+        <v>7850</v>
+      </c>
+      <c r="M11" s="372">
+        <v>1</v>
+      </c>
+      <c r="N11" s="24">
+        <f>D11*E11*M11</f>
+        <v>0.29364450825140531</v>
+      </c>
+      <c r="O11" s="373"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12" s="320"/>
+      <c r="B12" s="41"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="41"/>
+      <c r="I12" s="41"/>
+      <c r="J12" s="41"/>
+      <c r="K12" s="41"/>
+      <c r="L12" s="41"/>
+      <c r="M12" s="198" t="s">
+        <v>23</v>
+      </c>
+      <c r="N12" s="199" t="e">
+        <f>SUM(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="O12" s="313"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13" s="317"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="313"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14" s="345" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="203" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="203" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="203" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="203" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="203" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" s="203" t="s">
+        <v>44</v>
+      </c>
+      <c r="H14" s="203" t="s">
+        <v>45</v>
+      </c>
+      <c r="I14" s="203" t="s">
+        <v>23</v>
+      </c>
+      <c r="J14" s="41"/>
+      <c r="K14" s="41"/>
+      <c r="L14" s="41"/>
+      <c r="M14" s="41"/>
+      <c r="N14" s="41"/>
+      <c r="O14" s="313"/>
+    </row>
+    <row r="15" spans="1:15" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="380">
+        <v>10</v>
+      </c>
+      <c r="B15" s="125" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="381" t="s">
+        <v>398</v>
+      </c>
+      <c r="D15" s="18">
+        <v>1.3</v>
+      </c>
+      <c r="E15" s="125" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="382">
+        <v>1</v>
+      </c>
+      <c r="G15" s="383" t="s">
+        <v>404</v>
+      </c>
+      <c r="H15" s="384">
+        <f>1/2</f>
+        <v>0.5</v>
+      </c>
+      <c r="I15" s="136">
+        <f>D15*F15*H15</f>
+        <v>0.65</v>
+      </c>
+      <c r="J15" s="385"/>
+      <c r="K15" s="385"/>
+      <c r="L15" s="385"/>
+      <c r="M15" s="385"/>
+      <c r="N15" s="385"/>
+      <c r="O15" s="386"/>
+    </row>
+    <row r="16" spans="1:15" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="380">
+        <v>20</v>
+      </c>
+      <c r="B16" s="125" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="381" t="s">
+        <v>399</v>
+      </c>
+      <c r="D16" s="18">
+        <v>0.04</v>
+      </c>
+      <c r="E16" s="125" t="s">
+        <v>48</v>
+      </c>
+      <c r="F16" s="382">
+        <v>5.5</v>
+      </c>
+      <c r="G16" s="382" t="s">
+        <v>60</v>
+      </c>
+      <c r="H16" s="382">
+        <v>3</v>
+      </c>
+      <c r="I16" s="136">
+        <f t="shared" ref="I16:I19" si="0">D16*F16*H16</f>
+        <v>0.66</v>
+      </c>
+      <c r="J16" s="385"/>
+      <c r="K16" s="385"/>
+      <c r="L16" s="385"/>
+      <c r="M16" s="385"/>
+      <c r="N16" s="385"/>
+      <c r="O16" s="386"/>
+    </row>
+    <row r="17" spans="1:15" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="387">
+        <v>30</v>
+      </c>
+      <c r="B17" s="368" t="s">
+        <v>400</v>
+      </c>
+      <c r="C17" s="388" t="s">
+        <v>401</v>
+      </c>
+      <c r="D17" s="18">
+        <v>0.65</v>
+      </c>
+      <c r="E17" s="368" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" s="389">
+        <v>1</v>
+      </c>
+      <c r="G17" s="383" t="s">
+        <v>404</v>
+      </c>
+      <c r="H17" s="384">
+        <f>1/2</f>
+        <v>0.5</v>
+      </c>
+      <c r="I17" s="136">
+        <f t="shared" si="0"/>
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="J17" s="390"/>
+      <c r="K17" s="390"/>
+      <c r="L17" s="390"/>
+      <c r="M17" s="390"/>
+      <c r="N17" s="390"/>
+      <c r="O17" s="391"/>
+    </row>
+    <row r="18" spans="1:15" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="380">
+        <v>40</v>
+      </c>
+      <c r="B18" s="125" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="381" t="s">
+        <v>269</v>
+      </c>
+      <c r="D18" s="18">
+        <v>0.04</v>
+      </c>
+      <c r="E18" s="125" t="s">
+        <v>48</v>
+      </c>
+      <c r="F18" s="382">
+        <v>0.3</v>
+      </c>
+      <c r="G18" s="382" t="s">
+        <v>60</v>
+      </c>
+      <c r="H18" s="382">
+        <v>3</v>
+      </c>
+      <c r="I18" s="136">
+        <f t="shared" si="0"/>
+        <v>3.6000000000000004E-2</v>
+      </c>
+      <c r="J18" s="392"/>
+      <c r="K18" s="392"/>
+      <c r="L18" s="392"/>
+      <c r="M18" s="392"/>
+      <c r="N18" s="392"/>
+      <c r="O18" s="386"/>
+    </row>
+    <row r="19" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="380">
+        <v>50</v>
+      </c>
+      <c r="B19" s="388" t="s">
+        <v>402</v>
+      </c>
+      <c r="C19" s="388" t="s">
+        <v>403</v>
+      </c>
+      <c r="D19" s="18">
+        <v>0.35</v>
+      </c>
+      <c r="E19" s="368" t="s">
+        <v>99</v>
+      </c>
+      <c r="F19" s="389">
+        <v>1</v>
+      </c>
+      <c r="G19" s="89"/>
+      <c r="H19" s="382">
+        <v>1</v>
+      </c>
+      <c r="I19" s="136">
+        <f t="shared" si="0"/>
+        <v>0.35</v>
+      </c>
+      <c r="J19" s="393"/>
+      <c r="K19" s="393"/>
+      <c r="L19" s="393"/>
+      <c r="M19" s="393"/>
+      <c r="N19" s="393"/>
+      <c r="O19" s="394"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A20" s="320"/>
+      <c r="B20" s="41"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="41"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="208" t="s">
+        <v>23</v>
+      </c>
+      <c r="I20" s="209" t="e">
+        <f>SUM(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J20" s="41"/>
+      <c r="K20" s="41"/>
+      <c r="L20" s="41"/>
+      <c r="M20" s="41"/>
+      <c r="N20" s="41"/>
+      <c r="O20" s="313"/>
+    </row>
+    <row r="21" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="346"/>
+      <c r="B21" s="347"/>
+      <c r="C21" s="347"/>
+      <c r="D21" s="347"/>
+      <c r="E21" s="347"/>
+      <c r="F21" s="347"/>
+      <c r="G21" s="347"/>
+      <c r="H21" s="347"/>
+      <c r="I21" s="347"/>
+      <c r="J21" s="347"/>
+      <c r="K21" s="347"/>
+      <c r="L21" s="347"/>
+      <c r="M21" s="347"/>
+      <c r="N21" s="347"/>
+      <c r="O21" s="326"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" location="BOM!A1" display="Back to BOM"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="9" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K36" sqref="K36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>405</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="9" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:O15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" s="309"/>
+      <c r="B1" s="310"/>
+      <c r="C1" s="310"/>
+      <c r="D1" s="310"/>
+      <c r="E1" s="310"/>
+      <c r="F1" s="310"/>
+      <c r="G1" s="310"/>
+      <c r="H1" s="310"/>
+      <c r="I1" s="310"/>
+      <c r="J1" s="310"/>
+      <c r="K1" s="310"/>
+      <c r="L1" s="310"/>
+      <c r="M1" s="310"/>
+      <c r="N1" s="310"/>
+      <c r="O1" s="311"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" s="344" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="207" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="3">
+        <v>81</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="202" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" s="4" t="e">
+        <f>N11+I14</f>
+        <v>#REF!</v>
+      </c>
+      <c r="O2" s="313"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" s="344" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="202" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="202" t="s">
+        <v>7</v>
+      </c>
+      <c r="N3" s="5">
+        <v>1</v>
+      </c>
+      <c r="O3" s="313"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" s="344" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="202" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="202" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="313"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" s="344" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>389</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="202" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="202" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="202" t="s">
+        <v>13</v>
+      </c>
+      <c r="N5" s="4" t="e">
+        <f>N2*N3</f>
+        <v>#REF!</v>
+      </c>
+      <c r="O5" s="313"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" s="344" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="202" t="s">
+        <v>16</v>
+      </c>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="313"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7" s="344" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="313"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8" s="344" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="313"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" s="317"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="313"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" s="345" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="203" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="203" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="203" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="203" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="203" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="203" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" s="203" t="s">
+        <v>34</v>
+      </c>
+      <c r="I10" s="203" t="s">
+        <v>35</v>
+      </c>
+      <c r="J10" s="203" t="s">
+        <v>36</v>
+      </c>
+      <c r="K10" s="203" t="s">
+        <v>37</v>
+      </c>
+      <c r="L10" s="203" t="s">
+        <v>38</v>
+      </c>
+      <c r="M10" s="203" t="s">
+        <v>22</v>
+      </c>
+      <c r="N10" s="203" t="s">
+        <v>23</v>
+      </c>
+      <c r="O10" s="313"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11" s="320"/>
+      <c r="B11" s="41"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="41"/>
+      <c r="J11" s="41"/>
+      <c r="K11" s="41"/>
+      <c r="L11" s="41"/>
+      <c r="M11" s="198" t="s">
+        <v>23</v>
+      </c>
+      <c r="N11" s="199" t="e">
+        <f>SUM(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="O11" s="313"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12" s="317"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="313"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13" s="345" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="203" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="203" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="203" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="203" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" s="203" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="203" t="s">
+        <v>44</v>
+      </c>
+      <c r="H13" s="203" t="s">
+        <v>45</v>
+      </c>
+      <c r="I13" s="203" t="s">
+        <v>23</v>
+      </c>
+      <c r="J13" s="41"/>
+      <c r="K13" s="41"/>
+      <c r="L13" s="41"/>
+      <c r="M13" s="41"/>
+      <c r="N13" s="41"/>
+      <c r="O13" s="313"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14" s="320"/>
+      <c r="B14" s="41"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="208" t="s">
+        <v>23</v>
+      </c>
+      <c r="I14" s="209" t="e">
+        <f>SUM(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J14" s="41"/>
+      <c r="K14" s="41"/>
+      <c r="L14" s="41"/>
+      <c r="M14" s="41"/>
+      <c r="N14" s="41"/>
+      <c r="O14" s="313"/>
+    </row>
+    <row r="15" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="346"/>
+      <c r="B15" s="347"/>
+      <c r="C15" s="347"/>
+      <c r="D15" s="347"/>
+      <c r="E15" s="347"/>
+      <c r="F15" s="347"/>
+      <c r="G15" s="347"/>
+      <c r="H15" s="347"/>
+      <c r="I15" s="347"/>
+      <c r="J15" s="347"/>
+      <c r="K15" s="347"/>
+      <c r="L15" s="347"/>
+      <c r="M15" s="347"/>
+      <c r="N15" s="347"/>
+      <c r="O15" s="326"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" location="BOM!A1" display="Back to BOM"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -22012,7 +26087,7 @@
   <dimension ref="A2:N25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>